<commit_message>
Contenidos guion 5 grado 11
Contenidos Estado social de derecho
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion05/CS_11_05_CO_Escaleta.xlsx
+++ b/fuentes/contenidos/grado11/guion05/CS_11_05_CO_Escaleta.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Documents\Aula Planeta Colombia\Repositorios\CienciasSociales\fuentes\contenidos\grado11\guion05\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17175" windowHeight="7125"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5364"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
@@ -23,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="210">
   <si>
     <t>Asignatura</t>
   </si>
@@ -596,27 +591,12 @@
     <t>El Estado social de derecho en Colombia</t>
   </si>
   <si>
-    <t>¿Qué es el Estado social?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Interactivo que explica las características y fines del Estado social </t>
-  </si>
-  <si>
-    <t>Explicar los fines y características del Estado Social , plantear ejemplos</t>
-  </si>
-  <si>
     <t>Comprende las características de un Estado social de derecho</t>
   </si>
   <si>
-    <t>Actividad para reconocer carcaterísticas y fines de un Estado social de derecho</t>
-  </si>
-  <si>
     <t>Actividad para reconocer la razón de la independencia de poderes en Colombia</t>
   </si>
   <si>
-    <t>Comprende las importancia de la separación del poder público en Colombia</t>
-  </si>
-  <si>
     <t>La Constitución Política</t>
   </si>
   <si>
@@ -626,12 +606,6 @@
     <t>Recurso M5D-01</t>
   </si>
   <si>
-    <t>Identifica los derechos fundamentales contemplados en la Constitución Política de 1991</t>
-  </si>
-  <si>
-    <t>Actividad para conocer los derechos fundamentales de los colombianos</t>
-  </si>
-  <si>
     <t>La democracia</t>
   </si>
   <si>
@@ -651,6 +625,30 @@
   </si>
   <si>
     <t>CS_11_05_CO</t>
+  </si>
+  <si>
+    <t>Identifica los derechos de los colombianos</t>
+  </si>
+  <si>
+    <t>Actividad para conocer los derechos de las tres generaciones en Colombia</t>
+  </si>
+  <si>
+    <t>Asignado a Ana Hoyos.</t>
+  </si>
+  <si>
+    <t>Comprende la importancia de la separación del poder público en Colombia</t>
+  </si>
+  <si>
+    <t>Asignado a Sandra Cogua</t>
+  </si>
+  <si>
+    <t>¿Qué es el Estado Social de Derecho?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interactivo que explica las características y fines del Estado Social de Derecho </t>
+  </si>
+  <si>
+    <t>Actividad para reconocer carcaterísticas y fines de un Estado Social de Derecho</t>
   </si>
 </sst>
 </file>
@@ -811,7 +809,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -842,86 +840,84 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -973,7 +969,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1015,7 +1011,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1050,7 +1046,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1259,1345 +1255,1366 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U121"/>
+  <dimension ref="A1:U284"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3:B23"/>
+      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="15.4" customHeight="1" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.1328125" style="19" customWidth="1"/>
-    <col min="2" max="2" width="15.1328125" style="19" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" style="19" customWidth="1"/>
-    <col min="4" max="4" width="26.1328125" style="19" customWidth="1"/>
-    <col min="5" max="5" width="31" style="19" customWidth="1"/>
-    <col min="6" max="6" width="24.73046875" style="20" customWidth="1"/>
-    <col min="7" max="7" width="25.86328125" style="19" customWidth="1"/>
-    <col min="8" max="8" width="13.86328125" style="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11" style="20" customWidth="1"/>
-    <col min="10" max="10" width="34" style="19" customWidth="1"/>
-    <col min="11" max="11" width="3.73046875" style="19" customWidth="1"/>
-    <col min="12" max="12" width="17.3984375" style="19" customWidth="1"/>
-    <col min="13" max="13" width="3.59765625" style="19" customWidth="1"/>
-    <col min="14" max="14" width="8.6640625" style="19" customWidth="1"/>
-    <col min="15" max="15" width="37.86328125" style="20" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.46484375" style="20" customWidth="1"/>
-    <col min="17" max="17" width="6.9296875" style="20" customWidth="1"/>
-    <col min="18" max="18" width="6.6640625" style="19" customWidth="1"/>
-    <col min="19" max="19" width="14.796875" style="19" customWidth="1"/>
-    <col min="20" max="20" width="22.86328125" style="19" customWidth="1"/>
-    <col min="21" max="21" width="21.73046875" style="19" customWidth="1"/>
-    <col min="22" max="16384" width="11.3984375" style="19"/>
+    <col min="1" max="1" width="16.5546875" style="41" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" style="41" customWidth="1"/>
+    <col min="3" max="3" width="23" style="41" customWidth="1"/>
+    <col min="4" max="4" width="26.109375" style="41" customWidth="1"/>
+    <col min="5" max="5" width="31" style="41" customWidth="1"/>
+    <col min="6" max="6" width="24.6640625" style="45" customWidth="1"/>
+    <col min="7" max="7" width="25.88671875" style="41" customWidth="1"/>
+    <col min="8" max="8" width="13.88671875" style="45" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" style="45" customWidth="1"/>
+    <col min="10" max="10" width="34" style="41" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" style="41" customWidth="1"/>
+    <col min="12" max="12" width="17.44140625" style="41" customWidth="1"/>
+    <col min="13" max="14" width="9.33203125" style="41" customWidth="1"/>
+    <col min="15" max="15" width="37.88671875" style="45" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.5546875" style="45" customWidth="1"/>
+    <col min="17" max="17" width="20.44140625" style="45" customWidth="1"/>
+    <col min="18" max="18" width="23" style="41" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.6640625" style="41" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="25.88671875" style="41" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.6640625" style="41" customWidth="1"/>
+    <col min="22" max="16384" width="11.44140625" style="41"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="18" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="53" t="s">
+    <row r="1" spans="1:21" s="36" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="58" t="s">
+      <c r="C1" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="51" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="52" t="s">
+      <c r="E1" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="F1" s="49" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="54" t="s">
+      <c r="G1" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="51" t="s">
+      <c r="H1" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="51" t="s">
+      <c r="I1" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="56" t="s">
+      <c r="J1" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="55" t="s">
+      <c r="K1" s="53" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="54" t="s">
+      <c r="L1" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="57" t="s">
+      <c r="M1" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="57"/>
-      <c r="O1" s="48" t="s">
+      <c r="N1" s="55"/>
+      <c r="O1" s="46" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="48" t="s">
+      <c r="P1" s="46" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="49" t="s">
+      <c r="Q1" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="50" t="s">
+      <c r="R1" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="49" t="s">
+      <c r="S1" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="50" t="s">
+      <c r="T1" s="48" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="49" t="s">
+      <c r="U1" s="47" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="18" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="53"/>
-      <c r="B2" s="52"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="54"/>
+    <row r="2" spans="1:21" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="51"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="52"/>
       <c r="M2" s="17" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="48"/>
-      <c r="P2" s="48"/>
-      <c r="Q2" s="49"/>
-      <c r="R2" s="50"/>
-      <c r="S2" s="49"/>
-      <c r="T2" s="50"/>
-      <c r="U2" s="49"/>
-    </row>
-    <row r="3" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="21" t="s">
+      <c r="O2" s="46"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="47"/>
+      <c r="R2" s="48"/>
+      <c r="S2" s="47"/>
+      <c r="T2" s="48"/>
+      <c r="U2" s="47"/>
+    </row>
+    <row r="3" spans="1:21" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="37" t="s">
+        <v>201</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>123</v>
+      </c>
+      <c r="E3" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="F3" s="30"/>
+      <c r="G3" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="H3" s="30">
+        <v>1</v>
+      </c>
+      <c r="I3" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="K3" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="33"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q3" s="26">
+        <v>9</v>
+      </c>
+      <c r="R3" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="S3" s="40" t="s">
+        <v>127</v>
+      </c>
+      <c r="T3" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="U3" s="26" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="37" t="s">
+        <v>201</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>122</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="F4" s="20"/>
+      <c r="G4" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="H4" s="20">
+        <v>2</v>
+      </c>
+      <c r="I4" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="K4" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4" s="33"/>
+      <c r="N4" s="33"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q4" s="26">
+        <v>9</v>
+      </c>
+      <c r="R4" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="S4" s="40" t="s">
+        <v>127</v>
+      </c>
+      <c r="T4" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="U4" s="26" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>201</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>122</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="F5" s="20"/>
+      <c r="G5" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="H5" s="20">
+        <v>3</v>
+      </c>
+      <c r="I5" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="K5" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="M5" s="33"/>
+      <c r="N5" s="33"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q5" s="26">
+        <v>9</v>
+      </c>
+      <c r="R5" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="S5" s="40" t="s">
+        <v>127</v>
+      </c>
+      <c r="T5" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="U5" s="26" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="37" t="s">
+        <v>201</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>187</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="F6" s="20"/>
+      <c r="G6" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="H6" s="20">
+        <v>4</v>
+      </c>
+      <c r="I6" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="K6" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="M6" s="33"/>
+      <c r="N6" s="33"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q6" s="26">
+        <v>9</v>
+      </c>
+      <c r="R6" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="S6" s="40" t="s">
+        <v>127</v>
+      </c>
+      <c r="T6" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="U6" s="26" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>201</v>
+      </c>
+      <c r="C7" s="38" t="s">
+        <v>187</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="F7" s="20"/>
+      <c r="G7" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="H7" s="20">
+        <v>5</v>
+      </c>
+      <c r="I7" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="K7" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="M7" s="33"/>
+      <c r="N7" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="O7" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="P7" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q7" s="26">
+        <v>6</v>
+      </c>
+      <c r="R7" s="27" t="s">
+        <v>142</v>
+      </c>
+      <c r="S7" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="T7" s="43" t="s">
+        <v>144</v>
+      </c>
+      <c r="U7" s="26" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="37" t="s">
+        <v>201</v>
+      </c>
+      <c r="C8" s="38" t="s">
+        <v>187</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="F8" s="20"/>
+      <c r="G8" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="H8" s="20">
+        <v>6</v>
+      </c>
+      <c r="I8" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="22" t="s">
         <v>208</v>
       </c>
-      <c r="C3" s="23" t="s">
-        <v>122</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="E3" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="F3" s="24"/>
-      <c r="G3" s="25" t="s">
-        <v>125</v>
-      </c>
-      <c r="H3" s="24">
-        <v>1</v>
-      </c>
-      <c r="I3" s="24" t="s">
+      <c r="K8" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="M8" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="N8" s="33"/>
+      <c r="O8" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="P8" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="26" t="s">
-        <v>130</v>
-      </c>
-      <c r="K3" s="27" t="s">
+      <c r="Q8" s="26">
+        <v>6</v>
+      </c>
+      <c r="R8" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="S8" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="T8" s="43" t="s">
+        <v>148</v>
+      </c>
+      <c r="U8" s="26" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>201</v>
+      </c>
+      <c r="C9" s="38" t="s">
+        <v>187</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="F9" s="20"/>
+      <c r="G9" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="H9" s="20">
+        <v>7</v>
+      </c>
+      <c r="I9" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" s="22" t="s">
+        <v>209</v>
+      </c>
+      <c r="K9" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="L9" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="M9" s="33"/>
+      <c r="N9" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="O9" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="P9" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="30"/>
-      <c r="P3" s="30" t="s">
+      <c r="Q9" s="26">
+        <v>6</v>
+      </c>
+      <c r="R9" s="27" t="s">
+        <v>142</v>
+      </c>
+      <c r="S9" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="T9" s="43" t="s">
+        <v>151</v>
+      </c>
+      <c r="U9" s="26" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="37" t="s">
+        <v>201</v>
+      </c>
+      <c r="C10" s="38" t="s">
+        <v>187</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="F10" s="20"/>
+      <c r="G10" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="H10" s="20">
+        <v>8</v>
+      </c>
+      <c r="I10" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="K10" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="L10" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="M10" s="33"/>
+      <c r="N10" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="O10" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="P10" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="31">
+      <c r="Q10" s="26">
+        <v>6</v>
+      </c>
+      <c r="R10" s="27" t="s">
+        <v>142</v>
+      </c>
+      <c r="S10" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="T10" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="U10" s="26" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="37" t="s">
+        <v>201</v>
+      </c>
+      <c r="C11" s="38" t="s">
+        <v>187</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="F11" s="20"/>
+      <c r="G11" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="H11" s="20">
         <v>9</v>
       </c>
-      <c r="R3" s="32" t="s">
+      <c r="I11" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="K11" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="L11" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="M11" s="33"/>
+      <c r="N11" s="33"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q11" s="9">
+        <v>8</v>
+      </c>
+      <c r="R11" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="S3" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="T3" s="32" t="s">
-        <v>124</v>
-      </c>
-      <c r="U3" s="31" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="21" t="s">
+      <c r="S11" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="T11" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="U11" s="9" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="22" t="s">
-        <v>208</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>122</v>
-      </c>
-      <c r="D4" s="34" t="s">
-        <v>123</v>
-      </c>
-      <c r="E4" s="35" t="s">
-        <v>124</v>
-      </c>
-      <c r="F4" s="30"/>
-      <c r="G4" s="36" t="s">
-        <v>129</v>
-      </c>
-      <c r="H4" s="30">
-        <v>2</v>
-      </c>
-      <c r="I4" s="24" t="s">
+      <c r="B12" s="37" t="s">
+        <v>201</v>
+      </c>
+      <c r="C12" s="38" t="s">
+        <v>187</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="F12" s="20"/>
+      <c r="G12" s="21" t="s">
+        <v>205</v>
+      </c>
+      <c r="H12" s="20">
+        <v>10</v>
+      </c>
+      <c r="I12" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="37" t="s">
-        <v>131</v>
-      </c>
-      <c r="K4" s="27" t="s">
+      <c r="J12" s="22" t="s">
+        <v>191</v>
+      </c>
+      <c r="K12" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="L12" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="M12" s="33"/>
+      <c r="N12" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="O12" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="P12" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="L4" s="25" t="s">
+      <c r="Q12" s="9">
+        <v>6</v>
+      </c>
+      <c r="R12" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="S12" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="T12" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="U12" s="9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="37" t="s">
+        <v>201</v>
+      </c>
+      <c r="C13" s="38" t="s">
+        <v>187</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="E13" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="G13" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="H13" s="20">
+        <v>11</v>
+      </c>
+      <c r="I13" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="K13" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="L13" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="M13" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="N13" s="33"/>
+      <c r="O13" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="P13" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q13" s="26">
+        <v>6</v>
+      </c>
+      <c r="R13" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="S13" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="T13" s="43" t="s">
+        <v>163</v>
+      </c>
+      <c r="U13" s="26" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="37" t="s">
+        <v>201</v>
+      </c>
+      <c r="C14" s="38" t="s">
+        <v>187</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="E14" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="G14" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="H14" s="20">
+        <v>12</v>
+      </c>
+      <c r="I14" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14" s="22" t="s">
+        <v>203</v>
+      </c>
+      <c r="K14" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="L14" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="30"/>
-      <c r="P4" s="30" t="s">
+      <c r="M14" s="33"/>
+      <c r="N14" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="O14" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="P14" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="Q4" s="31">
-        <v>9</v>
-      </c>
-      <c r="R4" s="32" t="s">
-        <v>126</v>
-      </c>
-      <c r="S4" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="T4" s="38" t="s">
-        <v>132</v>
-      </c>
-      <c r="U4" s="31" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>208</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>122</v>
-      </c>
-      <c r="D5" s="34" t="s">
-        <v>123</v>
-      </c>
-      <c r="E5" s="35" t="s">
-        <v>133</v>
-      </c>
-      <c r="F5" s="30"/>
-      <c r="G5" s="39" t="s">
-        <v>134</v>
-      </c>
-      <c r="H5" s="30">
-        <v>3</v>
-      </c>
-      <c r="I5" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" s="37" t="s">
-        <v>135</v>
-      </c>
-      <c r="K5" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="L5" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
-      <c r="O5" s="30"/>
-      <c r="P5" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q5" s="31">
-        <v>9</v>
-      </c>
-      <c r="R5" s="32" t="s">
-        <v>126</v>
-      </c>
-      <c r="S5" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="T5" s="32" t="s">
-        <v>133</v>
-      </c>
-      <c r="U5" s="31" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>208</v>
-      </c>
-      <c r="C6" s="23" t="s">
-        <v>187</v>
-      </c>
-      <c r="D6" s="34" t="s">
-        <v>123</v>
-      </c>
-      <c r="E6" s="35" t="s">
-        <v>133</v>
-      </c>
-      <c r="F6" s="30"/>
-      <c r="G6" s="36" t="s">
-        <v>136</v>
-      </c>
-      <c r="H6" s="30">
-        <v>4</v>
-      </c>
-      <c r="I6" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="K6" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="L6" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
-      <c r="O6" s="30"/>
-      <c r="P6" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q6" s="31">
-        <v>9</v>
-      </c>
-      <c r="R6" s="32" t="s">
-        <v>126</v>
-      </c>
-      <c r="S6" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="T6" s="38" t="s">
-        <v>136</v>
-      </c>
-      <c r="U6" s="31" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>208</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>187</v>
-      </c>
-      <c r="D7" s="34" t="s">
-        <v>123</v>
-      </c>
-      <c r="E7" s="35" t="s">
-        <v>138</v>
-      </c>
-      <c r="F7" s="30"/>
-      <c r="G7" s="36" t="s">
-        <v>139</v>
-      </c>
-      <c r="H7" s="30">
-        <v>5</v>
-      </c>
-      <c r="I7" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="J7" s="40" t="s">
-        <v>140</v>
-      </c>
-      <c r="K7" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="L7" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="M7" s="29"/>
-      <c r="N7" s="29" t="s">
-        <v>121</v>
-      </c>
-      <c r="O7" s="30"/>
-      <c r="P7" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q7" s="31">
+      <c r="Q14" s="9">
         <v>6</v>
       </c>
-      <c r="R7" s="32" t="s">
+      <c r="R14" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="S7" s="31" t="s">
-        <v>143</v>
-      </c>
-      <c r="T7" s="41" t="s">
-        <v>144</v>
-      </c>
-      <c r="U7" s="31" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>208</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>187</v>
-      </c>
-      <c r="D8" s="34" t="s">
-        <v>188</v>
-      </c>
-      <c r="E8" s="35" t="s">
-        <v>141</v>
-      </c>
-      <c r="F8" s="30"/>
-      <c r="G8" s="39" t="s">
-        <v>190</v>
-      </c>
-      <c r="H8" s="30">
-        <v>6</v>
-      </c>
-      <c r="I8" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="J8" s="37" t="s">
-        <v>191</v>
-      </c>
-      <c r="K8" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="L8" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="M8" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="N8" s="29"/>
-      <c r="O8" s="30" t="s">
-        <v>192</v>
-      </c>
-      <c r="P8" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q8" s="31">
-        <v>6</v>
-      </c>
-      <c r="R8" s="32" t="s">
-        <v>146</v>
-      </c>
-      <c r="S8" s="31" t="s">
-        <v>147</v>
-      </c>
-      <c r="T8" s="41" t="s">
-        <v>148</v>
-      </c>
-      <c r="U8" s="31" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>208</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>187</v>
-      </c>
-      <c r="D9" s="34" t="s">
-        <v>188</v>
-      </c>
-      <c r="E9" s="35" t="s">
-        <v>150</v>
-      </c>
-      <c r="F9" s="30"/>
-      <c r="G9" s="36" t="s">
-        <v>193</v>
-      </c>
-      <c r="H9" s="30">
-        <v>7</v>
-      </c>
-      <c r="I9" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="J9" s="37" t="s">
-        <v>194</v>
-      </c>
-      <c r="K9" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="L9" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="M9" s="29"/>
-      <c r="N9" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="O9" s="30"/>
-      <c r="P9" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q9" s="31">
-        <v>6</v>
-      </c>
-      <c r="R9" s="32" t="s">
-        <v>142</v>
-      </c>
-      <c r="S9" s="31" t="s">
-        <v>143</v>
-      </c>
-      <c r="T9" s="41" t="s">
-        <v>151</v>
-      </c>
-      <c r="U9" s="31" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="22" t="s">
-        <v>208</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>187</v>
-      </c>
-      <c r="D10" s="34" t="s">
-        <v>188</v>
-      </c>
-      <c r="E10" s="35" t="s">
-        <v>138</v>
-      </c>
-      <c r="F10" s="30"/>
-      <c r="G10" s="36" t="s">
-        <v>152</v>
-      </c>
-      <c r="H10" s="30">
-        <v>8</v>
-      </c>
-      <c r="I10" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="J10" s="37" t="s">
-        <v>153</v>
-      </c>
-      <c r="K10" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="L10" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="M10" s="29"/>
-      <c r="N10" s="29" t="s">
-        <v>121</v>
-      </c>
-      <c r="O10" s="30"/>
-      <c r="P10" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q10" s="31">
-        <v>6</v>
-      </c>
-      <c r="R10" s="32" t="s">
-        <v>142</v>
-      </c>
-      <c r="S10" s="31" t="s">
-        <v>143</v>
-      </c>
-      <c r="T10" s="41" t="s">
-        <v>154</v>
-      </c>
-      <c r="U10" s="31" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>208</v>
-      </c>
-      <c r="C11" s="23" t="s">
-        <v>187</v>
-      </c>
-      <c r="D11" s="34" t="s">
-        <v>189</v>
-      </c>
-      <c r="E11" s="35" t="s">
-        <v>156</v>
-      </c>
-      <c r="F11" s="30"/>
-      <c r="G11" s="36" t="s">
-        <v>157</v>
-      </c>
-      <c r="H11" s="30">
-        <v>9</v>
-      </c>
-      <c r="I11" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="J11" s="37" t="s">
-        <v>158</v>
-      </c>
-      <c r="K11" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="L11" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="M11" s="29"/>
-      <c r="N11" s="29"/>
-      <c r="O11" s="30"/>
-      <c r="P11" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q11" s="42">
-        <v>8</v>
-      </c>
-      <c r="R11" s="43" t="s">
-        <v>126</v>
-      </c>
-      <c r="S11" s="42" t="s">
-        <v>197</v>
-      </c>
-      <c r="T11" s="43" t="s">
-        <v>157</v>
-      </c>
-      <c r="U11" s="42" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>208</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>187</v>
-      </c>
-      <c r="D12" s="34" t="s">
-        <v>189</v>
-      </c>
-      <c r="E12" s="35" t="s">
-        <v>156</v>
-      </c>
-      <c r="F12" s="30"/>
-      <c r="G12" s="36" t="s">
-        <v>196</v>
-      </c>
-      <c r="H12" s="30">
-        <v>10</v>
-      </c>
-      <c r="I12" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="J12" s="37" t="s">
-        <v>195</v>
-      </c>
-      <c r="K12" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="L12" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="M12" s="29"/>
-      <c r="N12" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="O12" s="30"/>
-      <c r="P12" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q12" s="42">
-        <v>6</v>
-      </c>
-      <c r="R12" s="43" t="s">
-        <v>142</v>
-      </c>
-      <c r="S12" s="42" t="s">
-        <v>143</v>
-      </c>
-      <c r="T12" s="44" t="s">
-        <v>199</v>
-      </c>
-      <c r="U12" s="42" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="22" t="s">
-        <v>208</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>187</v>
-      </c>
-      <c r="D13" s="34" t="s">
-        <v>189</v>
-      </c>
-      <c r="E13" s="45" t="s">
-        <v>159</v>
-      </c>
-      <c r="F13" s="30" t="s">
-        <v>160</v>
-      </c>
-      <c r="G13" s="36" t="s">
-        <v>161</v>
-      </c>
-      <c r="H13" s="30">
-        <v>11</v>
-      </c>
-      <c r="I13" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="J13" s="37" t="s">
-        <v>162</v>
-      </c>
-      <c r="K13" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="L13" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="M13" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="N13" s="29"/>
-      <c r="O13" s="30"/>
-      <c r="P13" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q13" s="31">
-        <v>6</v>
-      </c>
-      <c r="R13" s="32" t="s">
-        <v>146</v>
-      </c>
-      <c r="S13" s="31" t="s">
-        <v>147</v>
-      </c>
-      <c r="T13" s="41" t="s">
-        <v>163</v>
-      </c>
-      <c r="U13" s="31" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>208</v>
-      </c>
-      <c r="C14" s="23" t="s">
-        <v>187</v>
-      </c>
-      <c r="D14" s="34" t="s">
-        <v>189</v>
-      </c>
-      <c r="E14" s="45" t="s">
-        <v>159</v>
-      </c>
-      <c r="F14" s="30" t="s">
-        <v>160</v>
-      </c>
-      <c r="G14" s="36" t="s">
-        <v>200</v>
-      </c>
-      <c r="H14" s="30">
-        <v>12</v>
-      </c>
-      <c r="I14" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="J14" s="37" t="s">
-        <v>201</v>
-      </c>
-      <c r="K14" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="L14" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="M14" s="29"/>
-      <c r="N14" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="O14" s="30"/>
-      <c r="P14" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q14" s="42">
-        <v>6</v>
-      </c>
-      <c r="R14" s="43" t="s">
-        <v>142</v>
-      </c>
-      <c r="S14" s="42" t="s">
+      <c r="S14" s="9" t="s">
         <v>143</v>
       </c>
       <c r="T14" s="44" t="s">
         <v>151</v>
       </c>
-      <c r="U14" s="42" t="s">
+      <c r="U14" s="9" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="21" t="s">
+    <row r="15" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="22" t="s">
-        <v>208</v>
-      </c>
-      <c r="C15" s="23" t="s">
+      <c r="B15" s="37" t="s">
+        <v>201</v>
+      </c>
+      <c r="C15" s="38" t="s">
         <v>187</v>
       </c>
-      <c r="D15" s="34" t="s">
+      <c r="D15" s="18" t="s">
         <v>189</v>
       </c>
-      <c r="E15" s="45" t="s">
+      <c r="E15" s="28" t="s">
         <v>159</v>
       </c>
-      <c r="F15" s="30" t="s">
+      <c r="F15" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="G15" s="36" t="s">
+      <c r="G15" s="21" t="s">
         <v>165</v>
       </c>
-      <c r="H15" s="30">
+      <c r="H15" s="20">
         <v>13</v>
       </c>
-      <c r="I15" s="24" t="s">
+      <c r="I15" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="J15" s="37" t="s">
+      <c r="J15" s="22" t="s">
         <v>166</v>
       </c>
-      <c r="K15" s="27" t="s">
+      <c r="K15" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="L15" s="25" t="s">
+      <c r="L15" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="M15" s="29"/>
-      <c r="N15" s="29" t="s">
+      <c r="M15" s="33"/>
+      <c r="N15" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="O15" s="30"/>
-      <c r="P15" s="30" t="s">
+      <c r="O15" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="P15" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="Q15" s="31">
+      <c r="Q15" s="26">
         <v>6</v>
       </c>
-      <c r="R15" s="32" t="s">
+      <c r="R15" s="27" t="s">
         <v>142</v>
       </c>
-      <c r="S15" s="31" t="s">
+      <c r="S15" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="T15" s="41" t="s">
+      <c r="T15" s="43" t="s">
         <v>167</v>
       </c>
-      <c r="U15" s="31" t="s">
+      <c r="U15" s="26" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="21" t="s">
+    <row r="16" spans="1:21" ht="78" x14ac:dyDescent="0.3">
+      <c r="A16" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="22" t="s">
-        <v>208</v>
-      </c>
-      <c r="C16" s="23" t="s">
+      <c r="B16" s="37" t="s">
+        <v>201</v>
+      </c>
+      <c r="C16" s="38" t="s">
         <v>187</v>
       </c>
-      <c r="D16" s="34" t="s">
+      <c r="D16" s="18" t="s">
         <v>189</v>
       </c>
-      <c r="E16" s="45" t="s">
+      <c r="E16" s="28" t="s">
         <v>159</v>
       </c>
-      <c r="F16" s="46" t="s">
+      <c r="F16" s="29" t="s">
         <v>168</v>
       </c>
-      <c r="G16" s="36" t="s">
+      <c r="G16" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="H16" s="30">
+      <c r="H16" s="20">
         <v>14</v>
       </c>
-      <c r="I16" s="24" t="s">
+      <c r="I16" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="J16" s="37" t="s">
+      <c r="J16" s="22" t="s">
         <v>170</v>
       </c>
-      <c r="K16" s="27" t="s">
+      <c r="K16" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="L16" s="25" t="s">
+      <c r="L16" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="M16" s="29"/>
-      <c r="N16" s="29"/>
-      <c r="O16" s="30"/>
-      <c r="P16" s="30" t="s">
+      <c r="M16" s="33"/>
+      <c r="N16" s="33"/>
+      <c r="O16" s="20"/>
+      <c r="P16" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="Q16" s="42">
+      <c r="Q16" s="9">
         <v>8</v>
       </c>
-      <c r="R16" s="43" t="s">
+      <c r="R16" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="S16" s="42" t="s">
-        <v>202</v>
-      </c>
-      <c r="T16" s="43" t="s">
+      <c r="S16" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="T16" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="U16" s="42" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="21" t="s">
+      <c r="U16" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="22" t="s">
-        <v>208</v>
-      </c>
-      <c r="C17" s="23" t="s">
+      <c r="B17" s="37" t="s">
+        <v>201</v>
+      </c>
+      <c r="C17" s="38" t="s">
         <v>187</v>
       </c>
-      <c r="D17" s="47" t="s">
+      <c r="D17" s="25" t="s">
         <v>155</v>
       </c>
-      <c r="E17" s="45" t="s">
+      <c r="E17" s="28" t="s">
         <v>159</v>
       </c>
-      <c r="F17" s="46" t="s">
+      <c r="F17" s="29" t="s">
         <v>168</v>
       </c>
-      <c r="G17" s="36" t="s">
+      <c r="G17" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="H17" s="20">
+        <v>15</v>
+      </c>
+      <c r="I17" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="J17" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="K17" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="L17" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="M17" s="33"/>
+      <c r="N17" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="O17" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="P17" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q17" s="9">
+        <v>6</v>
+      </c>
+      <c r="R17" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="S17" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="T17" s="44" t="s">
+        <v>199</v>
+      </c>
+      <c r="U17" s="9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="37" t="s">
+        <v>201</v>
+      </c>
+      <c r="C18" s="38" t="s">
+        <v>187</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="F18" s="20"/>
+      <c r="G18" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="H18" s="20">
+        <v>16</v>
+      </c>
+      <c r="I18" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="J18" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="K18" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="L18" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="M18" s="33"/>
+      <c r="N18" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="O18" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="P18" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q18" s="26">
+        <v>6</v>
+      </c>
+      <c r="R18" s="27" t="s">
+        <v>142</v>
+      </c>
+      <c r="S18" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="T18" s="43" t="s">
+        <v>173</v>
+      </c>
+      <c r="U18" s="26" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="37" t="s">
+        <v>201</v>
+      </c>
+      <c r="C19" s="38" t="s">
+        <v>187</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="E19" s="19"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="H19" s="20">
+        <v>17</v>
+      </c>
+      <c r="I19" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="J19" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="K19" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="L19" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="M19" s="33"/>
+      <c r="N19" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="O19" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="H17" s="30">
-        <v>15</v>
-      </c>
-      <c r="I17" s="24" t="s">
+      <c r="P19" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q19" s="26">
+        <v>6</v>
+      </c>
+      <c r="R19" s="27" t="s">
+        <v>142</v>
+      </c>
+      <c r="S19" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="T19" s="43" t="s">
+        <v>176</v>
+      </c>
+      <c r="U19" s="26" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" ht="78" x14ac:dyDescent="0.3">
+      <c r="A20" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="37" t="s">
+        <v>201</v>
+      </c>
+      <c r="C20" s="38" t="s">
+        <v>187</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="E20" s="19"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="H20" s="20">
+        <v>18</v>
+      </c>
+      <c r="I20" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="37" t="s">
-        <v>205</v>
-      </c>
-      <c r="K17" s="27" t="s">
+      <c r="J20" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="K20" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="L20" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="M20" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="N20" s="33"/>
+      <c r="O20" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="P20" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="L17" s="25" t="s">
+      <c r="Q20" s="26">
+        <v>6</v>
+      </c>
+      <c r="R20" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="S20" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="T20" s="43" t="s">
+        <v>179</v>
+      </c>
+      <c r="U20" s="26" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="37" t="s">
+        <v>201</v>
+      </c>
+      <c r="C21" s="38" t="s">
+        <v>187</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="E21" s="19"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21" s="20">
+        <v>19</v>
+      </c>
+      <c r="I21" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="J21" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="K21" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="L21" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="M21" s="33"/>
+      <c r="N21" s="33"/>
+      <c r="O21" s="20"/>
+      <c r="P21" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q21" s="26"/>
+      <c r="R21" s="27"/>
+      <c r="S21" s="26"/>
+      <c r="T21" s="27"/>
+      <c r="U21" s="26"/>
+    </row>
+    <row r="22" spans="1:21" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A22" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="37" t="s">
+        <v>201</v>
+      </c>
+      <c r="C22" s="38" t="s">
+        <v>187</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="E22" s="19"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="H22" s="20">
+        <v>20</v>
+      </c>
+      <c r="I22" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="J22" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="K22" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="L22" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M22" s="33"/>
+      <c r="N22" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="O22" s="20"/>
+      <c r="P22" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q22" s="26">
+        <v>6</v>
+      </c>
+      <c r="R22" s="27" t="s">
+        <v>142</v>
+      </c>
+      <c r="S22" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="T22" s="43" t="s">
+        <v>184</v>
+      </c>
+      <c r="U22" s="26" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A23" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="37" t="s">
+        <v>201</v>
+      </c>
+      <c r="C23" s="38" t="s">
+        <v>187</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="E23" s="19"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="23" t="s">
+        <v>185</v>
+      </c>
+      <c r="H23" s="20">
+        <v>21</v>
+      </c>
+      <c r="I23" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="J23" s="24"/>
+      <c r="K23" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="L23" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="M17" s="29"/>
-      <c r="N17" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="O17" s="30"/>
-      <c r="P17" s="30" t="s">
+      <c r="M23" s="33"/>
+      <c r="N23" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="O23" s="20"/>
+      <c r="P23" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="Q17" s="42">
+      <c r="Q23" s="26">
         <v>6</v>
       </c>
-      <c r="R17" s="43" t="s">
+      <c r="R23" s="27" t="s">
         <v>142</v>
       </c>
-      <c r="S17" s="42" t="s">
+      <c r="S23" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="T17" s="44" t="s">
-        <v>206</v>
-      </c>
-      <c r="U17" s="42" t="s">
+      <c r="T23" s="43" t="s">
+        <v>186</v>
+      </c>
+      <c r="U23" s="26" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="22" t="s">
-        <v>208</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>187</v>
-      </c>
-      <c r="D18" s="47" t="s">
-        <v>155</v>
-      </c>
-      <c r="E18" s="35" t="s">
-        <v>138</v>
-      </c>
-      <c r="F18" s="30"/>
-      <c r="G18" s="36" t="s">
-        <v>171</v>
-      </c>
-      <c r="H18" s="30">
-        <v>16</v>
-      </c>
-      <c r="I18" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="J18" s="37" t="s">
-        <v>172</v>
-      </c>
-      <c r="K18" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="L18" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="M18" s="29"/>
-      <c r="N18" s="29" t="s">
-        <v>121</v>
-      </c>
-      <c r="O18" s="30"/>
-      <c r="P18" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q18" s="31">
-        <v>6</v>
-      </c>
-      <c r="R18" s="32" t="s">
-        <v>142</v>
-      </c>
-      <c r="S18" s="31" t="s">
-        <v>143</v>
-      </c>
-      <c r="T18" s="41" t="s">
-        <v>173</v>
-      </c>
-      <c r="U18" s="31" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="22" t="s">
-        <v>208</v>
-      </c>
-      <c r="C19" s="23" t="s">
-        <v>187</v>
-      </c>
-      <c r="D19" s="34" t="s">
-        <v>174</v>
-      </c>
-      <c r="E19" s="35"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="36" t="s">
-        <v>175</v>
-      </c>
-      <c r="H19" s="30">
-        <v>17</v>
-      </c>
-      <c r="I19" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="J19" s="37" t="s">
-        <v>207</v>
-      </c>
-      <c r="K19" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="L19" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="M19" s="29"/>
-      <c r="N19" s="29" t="s">
-        <v>120</v>
-      </c>
-      <c r="O19" s="30"/>
-      <c r="P19" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q19" s="31">
-        <v>6</v>
-      </c>
-      <c r="R19" s="32" t="s">
-        <v>142</v>
-      </c>
-      <c r="S19" s="31" t="s">
-        <v>143</v>
-      </c>
-      <c r="T19" s="41" t="s">
-        <v>176</v>
-      </c>
-      <c r="U19" s="31" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="22" t="s">
-        <v>208</v>
-      </c>
-      <c r="C20" s="23" t="s">
-        <v>187</v>
-      </c>
-      <c r="D20" s="34" t="s">
-        <v>174</v>
-      </c>
-      <c r="E20" s="35"/>
-      <c r="F20" s="30"/>
-      <c r="G20" s="36" t="s">
-        <v>177</v>
-      </c>
-      <c r="H20" s="30">
-        <v>18</v>
-      </c>
-      <c r="I20" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="J20" s="37" t="s">
-        <v>178</v>
-      </c>
-      <c r="K20" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="L20" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="M20" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="N20" s="29"/>
-      <c r="O20" s="30"/>
-      <c r="P20" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q20" s="31">
-        <v>6</v>
-      </c>
-      <c r="R20" s="32" t="s">
-        <v>146</v>
-      </c>
-      <c r="S20" s="31" t="s">
-        <v>147</v>
-      </c>
-      <c r="T20" s="41" t="s">
-        <v>179</v>
-      </c>
-      <c r="U20" s="31" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" s="22" t="s">
-        <v>208</v>
-      </c>
-      <c r="C21" s="23" t="s">
-        <v>187</v>
-      </c>
-      <c r="D21" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="E21" s="35"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="H21" s="30">
-        <v>19</v>
-      </c>
-      <c r="I21" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="J21" s="37" t="s">
-        <v>181</v>
-      </c>
-      <c r="K21" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="L21" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="M21" s="29"/>
-      <c r="N21" s="29"/>
-      <c r="O21" s="30"/>
-      <c r="P21" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q21" s="31"/>
-      <c r="R21" s="32"/>
-      <c r="S21" s="31"/>
-      <c r="T21" s="32"/>
-      <c r="U21" s="31"/>
-    </row>
-    <row r="22" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22" s="22" t="s">
-        <v>208</v>
-      </c>
-      <c r="C22" s="23" t="s">
-        <v>187</v>
-      </c>
-      <c r="D22" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="E22" s="35"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="39" t="s">
-        <v>182</v>
-      </c>
-      <c r="H22" s="30">
-        <v>20</v>
-      </c>
-      <c r="I22" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="J22" s="37" t="s">
-        <v>183</v>
-      </c>
-      <c r="K22" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="L22" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="M22" s="29"/>
-      <c r="N22" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="O22" s="30"/>
-      <c r="P22" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q22" s="31">
-        <v>6</v>
-      </c>
-      <c r="R22" s="32" t="s">
-        <v>142</v>
-      </c>
-      <c r="S22" s="31" t="s">
-        <v>143</v>
-      </c>
-      <c r="T22" s="41" t="s">
-        <v>184</v>
-      </c>
-      <c r="U22" s="31" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23" s="22" t="s">
-        <v>208</v>
-      </c>
-      <c r="C23" s="23" t="s">
-        <v>187</v>
-      </c>
-      <c r="D23" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="E23" s="35"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="39" t="s">
-        <v>185</v>
-      </c>
-      <c r="H23" s="30">
-        <v>21</v>
-      </c>
-      <c r="I23" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="J23" s="40"/>
-      <c r="K23" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="L23" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="M23" s="29"/>
-      <c r="N23" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="O23" s="30"/>
-      <c r="P23" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q23" s="31">
-        <v>6</v>
-      </c>
-      <c r="R23" s="32" t="s">
-        <v>142</v>
-      </c>
-      <c r="S23" s="31" t="s">
-        <v>143</v>
-      </c>
-      <c r="T23" s="41" t="s">
-        <v>186</v>
-      </c>
-      <c r="U23" s="31" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="12"/>
       <c r="C24" s="13"/>
@@ -2620,7 +2637,7 @@
       <c r="T24" s="11"/>
       <c r="U24" s="9"/>
     </row>
-    <row r="25" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="12"/>
       <c r="C25" s="13"/>
@@ -2643,7 +2660,7 @@
       <c r="T25" s="11"/>
       <c r="U25" s="9"/>
     </row>
-    <row r="26" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="12"/>
       <c r="C26" s="13"/>
@@ -2666,7 +2683,7 @@
       <c r="T26" s="11"/>
       <c r="U26" s="9"/>
     </row>
-    <row r="27" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="12"/>
       <c r="C27" s="13"/>
@@ -2689,7 +2706,7 @@
       <c r="T27" s="11"/>
       <c r="U27" s="9"/>
     </row>
-    <row r="28" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="12"/>
       <c r="C28" s="13"/>
@@ -2712,7 +2729,7 @@
       <c r="T28" s="11"/>
       <c r="U28" s="9"/>
     </row>
-    <row r="29" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="12"/>
       <c r="C29" s="13"/>
@@ -2735,7 +2752,7 @@
       <c r="T29" s="11"/>
       <c r="U29" s="9"/>
     </row>
-    <row r="30" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="12"/>
       <c r="C30" s="13"/>
@@ -2758,7 +2775,7 @@
       <c r="T30" s="11"/>
       <c r="U30" s="9"/>
     </row>
-    <row r="31" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="12"/>
       <c r="C31" s="13"/>
@@ -2781,7 +2798,7 @@
       <c r="T31" s="11"/>
       <c r="U31" s="9"/>
     </row>
-    <row r="32" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="12"/>
       <c r="C32" s="13"/>
@@ -2804,7 +2821,7 @@
       <c r="T32" s="11"/>
       <c r="U32" s="9"/>
     </row>
-    <row r="33" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="12"/>
       <c r="C33" s="13"/>
@@ -2827,7 +2844,7 @@
       <c r="T33" s="11"/>
       <c r="U33" s="9"/>
     </row>
-    <row r="34" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="B34" s="12"/>
       <c r="C34" s="13"/>
@@ -2850,7 +2867,7 @@
       <c r="T34" s="11"/>
       <c r="U34" s="9"/>
     </row>
-    <row r="35" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" s="12"/>
       <c r="C35" s="13"/>
@@ -2873,7 +2890,7 @@
       <c r="T35" s="11"/>
       <c r="U35" s="9"/>
     </row>
-    <row r="36" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="12"/>
       <c r="C36" s="13"/>
@@ -2896,7 +2913,7 @@
       <c r="T36" s="11"/>
       <c r="U36" s="9"/>
     </row>
-    <row r="37" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="12"/>
       <c r="C37" s="13"/>
@@ -2919,7 +2936,7 @@
       <c r="T37" s="11"/>
       <c r="U37" s="9"/>
     </row>
-    <row r="38" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" s="12"/>
       <c r="C38" s="13"/>
@@ -2942,7 +2959,7 @@
       <c r="T38" s="11"/>
       <c r="U38" s="9"/>
     </row>
-    <row r="39" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
       <c r="B39" s="12"/>
       <c r="C39" s="13"/>
@@ -2965,7 +2982,7 @@
       <c r="T39" s="11"/>
       <c r="U39" s="9"/>
     </row>
-    <row r="40" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
       <c r="B40" s="12"/>
       <c r="C40" s="13"/>
@@ -2988,7 +3005,7 @@
       <c r="T40" s="11"/>
       <c r="U40" s="9"/>
     </row>
-    <row r="41" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="3"/>
       <c r="B41" s="12"/>
       <c r="C41" s="13"/>
@@ -3011,7 +3028,7 @@
       <c r="T41" s="11"/>
       <c r="U41" s="9"/>
     </row>
-    <row r="42" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
       <c r="B42" s="12"/>
       <c r="C42" s="13"/>
@@ -3034,7 +3051,7 @@
       <c r="T42" s="11"/>
       <c r="U42" s="9"/>
     </row>
-    <row r="43" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="3"/>
       <c r="B43" s="12"/>
       <c r="C43" s="13"/>
@@ -3057,7 +3074,7 @@
       <c r="T43" s="11"/>
       <c r="U43" s="9"/>
     </row>
-    <row r="44" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="3"/>
       <c r="B44" s="12"/>
       <c r="C44" s="13"/>
@@ -3080,7 +3097,7 @@
       <c r="T44" s="11"/>
       <c r="U44" s="9"/>
     </row>
-    <row r="45" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="3"/>
       <c r="B45" s="12"/>
       <c r="C45" s="13"/>
@@ -3103,7 +3120,7 @@
       <c r="T45" s="11"/>
       <c r="U45" s="9"/>
     </row>
-    <row r="46" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="3"/>
       <c r="B46" s="12"/>
       <c r="C46" s="13"/>
@@ -3126,7 +3143,7 @@
       <c r="T46" s="11"/>
       <c r="U46" s="9"/>
     </row>
-    <row r="47" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="3"/>
       <c r="B47" s="12"/>
       <c r="C47" s="13"/>
@@ -3149,7 +3166,7 @@
       <c r="T47" s="11"/>
       <c r="U47" s="9"/>
     </row>
-    <row r="48" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="3"/>
       <c r="B48" s="12"/>
       <c r="C48" s="13"/>
@@ -3172,7 +3189,7 @@
       <c r="T48" s="11"/>
       <c r="U48" s="9"/>
     </row>
-    <row r="49" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="3"/>
       <c r="B49" s="12"/>
       <c r="C49" s="13"/>
@@ -3195,7 +3212,7 @@
       <c r="T49" s="11"/>
       <c r="U49" s="9"/>
     </row>
-    <row r="50" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="3"/>
       <c r="B50" s="12"/>
       <c r="C50" s="13"/>
@@ -3218,7 +3235,7 @@
       <c r="T50" s="11"/>
       <c r="U50" s="9"/>
     </row>
-    <row r="51" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" s="3"/>
       <c r="B51" s="12"/>
       <c r="C51" s="13"/>
@@ -3241,7 +3258,7 @@
       <c r="T51" s="11"/>
       <c r="U51" s="9"/>
     </row>
-    <row r="52" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="3"/>
       <c r="B52" s="12"/>
       <c r="C52" s="13"/>
@@ -3264,7 +3281,7 @@
       <c r="T52" s="11"/>
       <c r="U52" s="9"/>
     </row>
-    <row r="53" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="3"/>
       <c r="B53" s="12"/>
       <c r="C53" s="13"/>
@@ -3287,7 +3304,7 @@
       <c r="T53" s="11"/>
       <c r="U53" s="9"/>
     </row>
-    <row r="54" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="3"/>
       <c r="B54" s="12"/>
       <c r="C54" s="13"/>
@@ -3310,7 +3327,7 @@
       <c r="T54" s="11"/>
       <c r="U54" s="9"/>
     </row>
-    <row r="55" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A55" s="3"/>
       <c r="B55" s="12"/>
       <c r="C55" s="13"/>
@@ -3333,7 +3350,7 @@
       <c r="T55" s="11"/>
       <c r="U55" s="9"/>
     </row>
-    <row r="56" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" s="3"/>
       <c r="B56" s="12"/>
       <c r="C56" s="13"/>
@@ -3356,7 +3373,7 @@
       <c r="T56" s="11"/>
       <c r="U56" s="9"/>
     </row>
-    <row r="57" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" s="3"/>
       <c r="B57" s="12"/>
       <c r="C57" s="13"/>
@@ -3379,7 +3396,7 @@
       <c r="T57" s="11"/>
       <c r="U57" s="9"/>
     </row>
-    <row r="58" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="3"/>
       <c r="B58" s="12"/>
       <c r="C58" s="13"/>
@@ -3402,7 +3419,7 @@
       <c r="T58" s="11"/>
       <c r="U58" s="9"/>
     </row>
-    <row r="59" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="3"/>
       <c r="B59" s="12"/>
       <c r="C59" s="13"/>
@@ -3425,7 +3442,7 @@
       <c r="T59" s="11"/>
       <c r="U59" s="9"/>
     </row>
-    <row r="60" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" s="3"/>
       <c r="B60" s="12"/>
       <c r="C60" s="13"/>
@@ -3448,7 +3465,7 @@
       <c r="T60" s="11"/>
       <c r="U60" s="9"/>
     </row>
-    <row r="61" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="3"/>
       <c r="B61" s="12"/>
       <c r="C61" s="13"/>
@@ -3471,7 +3488,7 @@
       <c r="T61" s="11"/>
       <c r="U61" s="9"/>
     </row>
-    <row r="62" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" s="3"/>
       <c r="B62" s="12"/>
       <c r="C62" s="13"/>
@@ -3494,7 +3511,7 @@
       <c r="T62" s="11"/>
       <c r="U62" s="9"/>
     </row>
-    <row r="63" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A63" s="3"/>
       <c r="B63" s="12"/>
       <c r="C63" s="13"/>
@@ -3517,7 +3534,7 @@
       <c r="T63" s="11"/>
       <c r="U63" s="9"/>
     </row>
-    <row r="64" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A64" s="3"/>
       <c r="B64" s="12"/>
       <c r="C64" s="13"/>
@@ -3540,7 +3557,7 @@
       <c r="T64" s="11"/>
       <c r="U64" s="9"/>
     </row>
-    <row r="65" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A65" s="3"/>
       <c r="B65" s="12"/>
       <c r="C65" s="13"/>
@@ -3563,7 +3580,7 @@
       <c r="T65" s="11"/>
       <c r="U65" s="9"/>
     </row>
-    <row r="66" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="3"/>
       <c r="B66" s="12"/>
       <c r="C66" s="13"/>
@@ -3586,7 +3603,7 @@
       <c r="T66" s="11"/>
       <c r="U66" s="9"/>
     </row>
-    <row r="67" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A67" s="3"/>
       <c r="B67" s="12"/>
       <c r="C67" s="13"/>
@@ -3609,7 +3626,7 @@
       <c r="T67" s="11"/>
       <c r="U67" s="9"/>
     </row>
-    <row r="68" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A68" s="3"/>
       <c r="B68" s="12"/>
       <c r="C68" s="13"/>
@@ -3632,7 +3649,7 @@
       <c r="T68" s="11"/>
       <c r="U68" s="9"/>
     </row>
-    <row r="69" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A69" s="3"/>
       <c r="B69" s="12"/>
       <c r="C69" s="13"/>
@@ -3655,7 +3672,7 @@
       <c r="T69" s="11"/>
       <c r="U69" s="9"/>
     </row>
-    <row r="70" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A70" s="3"/>
       <c r="B70" s="12"/>
       <c r="C70" s="13"/>
@@ -3678,191 +3695,367 @@
       <c r="T70" s="11"/>
       <c r="U70" s="9"/>
     </row>
-    <row r="85" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A85" s="19" t="s">
+    <row r="72" spans="1:21" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="73" spans="1:21" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="74" spans="1:21" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="75" spans="1:21" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="76" spans="1:21" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="77" spans="1:21" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="78" spans="1:21" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="79" spans="1:21" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="80" spans="1:21" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="81" spans="1:1" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="82" spans="1:1" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="83" spans="1:1" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="84" spans="1:1" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="85" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="41" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="86" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A86" s="19" t="s">
+    <row r="86" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="41" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="87" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A87" s="19" t="s">
+    <row r="87" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="41" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="88" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A88" s="19" t="s">
+    <row r="88" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="41" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="89" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A89" s="19" t="s">
+    <row r="89" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="41" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="90" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A90" s="19" t="s">
+    <row r="90" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="41" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="91" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A91" s="19" t="s">
+    <row r="91" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="41" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="92" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A92" s="19" t="s">
+    <row r="92" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="41" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="93" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A93" s="19" t="s">
+    <row r="93" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="41" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="94" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A94" s="19" t="s">
+    <row r="94" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="41" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="95" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A95" s="19" t="s">
+    <row r="95" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="41" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="96" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A96" s="19" t="s">
+    <row r="96" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="41" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="97" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A97" s="19" t="s">
+    <row r="97" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="41" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="98" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A98" s="19" t="s">
+    <row r="98" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="41" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="99" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A99" s="19" t="s">
+    <row r="99" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="41" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="100" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A100" s="19" t="s">
+    <row r="100" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="41" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="101" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A101" s="19" t="s">
+    <row r="101" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="41" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="102" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A102" s="19" t="s">
+    <row r="102" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="41" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="103" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A103" s="19" t="s">
+    <row r="103" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="41" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="104" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A104" s="19" t="s">
+    <row r="104" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="41" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="105" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A105" s="19" t="s">
+    <row r="105" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="41" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="106" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A106" s="19" t="s">
+    <row r="106" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="41" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="107" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A107" s="19" t="s">
+    <row r="107" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="41" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="108" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A108" s="19" t="s">
+    <row r="108" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="41" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="109" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A109" s="19" t="s">
+    <row r="109" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="41" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="110" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A110" s="19" t="s">
+    <row r="110" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="41" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="111" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A111" s="19" t="s">
+    <row r="111" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="41" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="112" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A112" s="19" t="s">
+    <row r="112" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="41" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="113" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A113" s="19" t="s">
+    <row r="113" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="41" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="114" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A114" s="19" t="s">
+    <row r="114" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="41" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="115" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A115" s="19" t="s">
+    <row r="115" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="41" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="116" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A116" s="19" t="s">
+    <row r="116" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="41" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="117" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A117" s="19" t="s">
+    <row r="117" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="41" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="118" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A118" s="19" t="s">
+    <row r="118" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A118" s="41" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="119" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A119" s="19" t="s">
+    <row r="119" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="41" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="120" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A120" s="19" t="s">
+    <row r="120" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="41" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="121" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A121" s="19" t="s">
+    <row r="121" spans="1:1" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="41" t="s">
         <v>115</v>
       </c>
     </row>
+    <row r="122" spans="1:1" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="123" spans="1:1" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="124" spans="1:1" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="125" spans="1:1" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="126" spans="1:1" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="127" spans="1:1" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="128" spans="1:1" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="129" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="130" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="131" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="132" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="133" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="134" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="135" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="136" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="137" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="138" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="139" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="140" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="141" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="142" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="143" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="144" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="145" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="146" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="147" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="148" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="149" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="150" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="151" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="152" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="153" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="154" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="155" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="156" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="157" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="158" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="159" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="160" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="161" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="162" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="163" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="164" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="165" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="166" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="167" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="168" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="169" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="170" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="171" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="172" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="173" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="174" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="175" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="176" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="177" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="178" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="179" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="180" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="181" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="182" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="183" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="184" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="185" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="186" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="187" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="188" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="189" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="190" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="191" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="192" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="193" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="194" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="195" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="196" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="197" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="198" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="199" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="200" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="201" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="202" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="203" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="204" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="205" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="206" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="207" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="208" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="209" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="210" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="211" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="212" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="213" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="214" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="215" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="216" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="217" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="218" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="219" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="220" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="221" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="222" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="223" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="224" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="225" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="226" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="227" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="228" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="229" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="230" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="231" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="232" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="233" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="234" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="235" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="236" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="237" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="238" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="239" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="240" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="241" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="242" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="243" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="244" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="245" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="246" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="247" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="248" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="249" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="250" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="251" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="252" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="253" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="254" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="255" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="256" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="257" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="258" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="259" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="260" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="261" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="262" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="263" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="264" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="265" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="266" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="267" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="268" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="269" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="270" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="271" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="272" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="273" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="274" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="275" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="276" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="277" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="278" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="279" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="280" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="281" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="282" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="283" hidden="1" x14ac:dyDescent="0.3"/>
+    <row r="284" hidden="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <autoFilter ref="A1:U2">
     <filterColumn colId="12" showButton="0"/>
@@ -3938,27 +4131,27 @@
       <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.86328125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" style="1" customWidth="1"/>
     <col min="4" max="4" width="34" style="1" customWidth="1"/>
-    <col min="5" max="5" width="34.86328125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.59765625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="34.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.5546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="18" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.73046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.73046875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.59765625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5546875" style="1" customWidth="1"/>
     <col min="12" max="12" width="17" style="1" customWidth="1"/>
-    <col min="13" max="13" width="11.3984375" style="1"/>
-    <col min="14" max="14" width="24.265625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="69.86328125" style="1" hidden="1" customWidth="1"/>
-    <col min="16" max="16384" width="11.3984375" style="1"/>
+    <col min="13" max="13" width="11.44140625" style="1"/>
+    <col min="14" max="14" width="24.33203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="69.88671875" style="1" hidden="1" customWidth="1"/>
+    <col min="16" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -3975,7 +4168,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -3999,7 +4192,7 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -4018,7 +4211,7 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -4037,7 +4230,7 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
@@ -4053,7 +4246,7 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
@@ -4070,7 +4263,7 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
@@ -4087,7 +4280,7 @@
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -4102,7 +4295,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -4117,7 +4310,7 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -4132,7 +4325,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -4147,7 +4340,7 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -4162,7 +4355,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -4177,7 +4370,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -4192,7 +4385,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -4207,7 +4400,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -4222,7 +4415,7 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="1" t="s">
@@ -4236,7 +4429,7 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="1" t="s">
@@ -4250,7 +4443,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="1" t="s">
@@ -4264,7 +4457,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="1" t="s">
@@ -4278,7 +4471,7 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="21" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -4293,7 +4486,7 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="22" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -4308,7 +4501,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="23" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -4323,7 +4516,7 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="24" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -4338,7 +4531,7 @@
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
     </row>
-    <row r="25" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="25" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -4353,7 +4546,7 @@
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="26" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -4368,7 +4561,7 @@
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
     </row>
-    <row r="27" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="27" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -4383,7 +4576,7 @@
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
     </row>
-    <row r="28" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="28" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -4398,7 +4591,7 @@
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="29" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -4413,7 +4606,7 @@
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
     </row>
-    <row r="30" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="30" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -4428,7 +4621,7 @@
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
     </row>
-    <row r="31" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="31" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -4443,7 +4636,7 @@
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
     </row>
-    <row r="32" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="32" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -4458,7 +4651,7 @@
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
     </row>
-    <row r="33" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="33" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -4473,7 +4666,7 @@
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
     </row>
-    <row r="34" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="34" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -4488,7 +4681,7 @@
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
     </row>
-    <row r="35" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="35" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -4503,7 +4696,7 @@
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
     </row>
-    <row r="36" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="36" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -4518,7 +4711,7 @@
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
     </row>
-    <row r="37" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="37" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -4533,7 +4726,7 @@
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
     </row>
-    <row r="38" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="38" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -4548,7 +4741,7 @@
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
     </row>
-    <row r="39" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="39" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -4563,7 +4756,7 @@
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
     </row>
-    <row r="40" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="40" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -4578,7 +4771,7 @@
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
     </row>
-    <row r="41" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="41" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -4593,7 +4786,7 @@
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
     </row>
-    <row r="42" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="42" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -4608,7 +4801,7 @@
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
     </row>
-    <row r="43" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="43" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -4623,7 +4816,7 @@
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
     </row>
-    <row r="44" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="44" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -4638,7 +4831,7 @@
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
     </row>
-    <row r="45" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="45" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -4653,7 +4846,7 @@
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
     </row>
-    <row r="46" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="46" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -4668,7 +4861,7 @@
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
     </row>
-    <row r="47" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="47" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -4683,7 +4876,7 @@
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
     </row>
-    <row r="48" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="48" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -4698,7 +4891,7 @@
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
     </row>
-    <row r="49" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="49" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -4710,7 +4903,7 @@
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
     </row>
-    <row r="50" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="50" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
@@ -4722,7 +4915,7 @@
       <c r="K50" s="2"/>
       <c r="L50" s="2"/>
     </row>
-    <row r="51" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="51" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
@@ -4735,7 +4928,7 @@
       <c r="K51" s="2"/>
       <c r="L51" s="2"/>
     </row>
-    <row r="52" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="52" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -4748,7 +4941,7 @@
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
     </row>
-    <row r="53" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="53" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -4761,7 +4954,7 @@
       <c r="K53" s="2"/>
       <c r="L53" s="2"/>
     </row>
-    <row r="54" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="54" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
@@ -4774,7 +4967,7 @@
       <c r="K54" s="2"/>
       <c r="L54" s="2"/>
     </row>
-    <row r="55" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="55" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
@@ -4787,7 +4980,7 @@
       <c r="K55" s="2"/>
       <c r="L55" s="2"/>
     </row>
-    <row r="56" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="56" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
@@ -4800,7 +4993,7 @@
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
     </row>
-    <row r="57" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="57" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
@@ -4813,7 +5006,7 @@
       <c r="K57" s="2"/>
       <c r="L57" s="2"/>
     </row>
-    <row r="58" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="58" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
@@ -4826,7 +5019,7 @@
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
     </row>
-    <row r="59" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="59" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
@@ -4839,7 +5032,7 @@
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
     </row>
-    <row r="60" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="60" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -4852,7 +5045,7 @@
       <c r="K60" s="2"/>
       <c r="L60" s="2"/>
     </row>
-    <row r="61" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="61" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
@@ -4865,7 +5058,7 @@
       <c r="K61" s="2"/>
       <c r="L61" s="2"/>
     </row>
-    <row r="62" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="62" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
@@ -4878,7 +5071,7 @@
       <c r="K62" s="2"/>
       <c r="L62" s="2"/>
     </row>
-    <row r="63" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="63" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
@@ -4891,7 +5084,7 @@
       <c r="K63" s="2"/>
       <c r="L63" s="2"/>
     </row>
-    <row r="64" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="64" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
@@ -4904,7 +5097,7 @@
       <c r="K64" s="2"/>
       <c r="L64" s="2"/>
     </row>
-    <row r="65" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
@@ -4917,7 +5110,7 @@
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
     </row>
-    <row r="66" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
@@ -4930,7 +5123,7 @@
       <c r="K66" s="2"/>
       <c r="L66" s="2"/>
     </row>
-    <row r="67" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
@@ -4943,7 +5136,7 @@
       <c r="K67" s="2"/>
       <c r="L67" s="2"/>
     </row>
-    <row r="68" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
@@ -4956,7 +5149,7 @@
       <c r="K68" s="2"/>
       <c r="L68" s="2"/>
     </row>
-    <row r="69" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
@@ -4969,7 +5162,7 @@
       <c r="K69" s="2"/>
       <c r="L69" s="2"/>
     </row>
-    <row r="70" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
@@ -4982,7 +5175,7 @@
       <c r="K70" s="2"/>
       <c r="L70" s="2"/>
     </row>
-    <row r="71" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -4996,7 +5189,7 @@
       <c r="K71" s="2"/>
       <c r="L71" s="2"/>
     </row>
-    <row r="72" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -5010,7 +5203,7 @@
       <c r="K72" s="2"/>
       <c r="L72" s="2"/>
     </row>
-    <row r="73" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -5024,7 +5217,7 @@
       <c r="K73" s="2"/>
       <c r="L73" s="2"/>
     </row>
-    <row r="74" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -5038,7 +5231,7 @@
       <c r="K74" s="2"/>
       <c r="L74" s="2"/>
     </row>
-    <row r="75" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -5052,7 +5245,7 @@
       <c r="K75" s="2"/>
       <c r="L75" s="2"/>
     </row>
-    <row r="76" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -5066,7 +5259,7 @@
       <c r="K76" s="2"/>
       <c r="L76" s="2"/>
     </row>
-    <row r="77" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -5080,7 +5273,7 @@
       <c r="K77" s="2"/>
       <c r="L77" s="2"/>
     </row>
-    <row r="78" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -5094,7 +5287,7 @@
       <c r="K78" s="2"/>
       <c r="L78" s="2"/>
     </row>
-    <row r="79" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -5108,7 +5301,7 @@
       <c r="K79" s="2"/>
       <c r="L79" s="2"/>
     </row>
-    <row r="80" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -5122,7 +5315,7 @@
       <c r="K80" s="2"/>
       <c r="L80" s="2"/>
     </row>
-    <row r="81" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -5136,7 +5329,7 @@
       <c r="K81" s="2"/>
       <c r="L81" s="2"/>
     </row>
-    <row r="82" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -5150,7 +5343,7 @@
       <c r="K82" s="2"/>
       <c r="L82" s="2"/>
     </row>
-    <row r="83" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -5164,7 +5357,7 @@
       <c r="K83" s="2"/>
       <c r="L83" s="2"/>
     </row>
-    <row r="84" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -5178,7 +5371,7 @@
       <c r="K84" s="2"/>
       <c r="L84" s="2"/>
     </row>
-    <row r="85" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -5192,7 +5385,7 @@
       <c r="K85" s="2"/>
       <c r="L85" s="2"/>
     </row>
-    <row r="86" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="86" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -5206,7 +5399,7 @@
       <c r="K86" s="2"/>
       <c r="L86" s="2"/>
     </row>
-    <row r="87" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="87" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -5220,7 +5413,7 @@
       <c r="K87" s="2"/>
       <c r="L87" s="2"/>
     </row>
-    <row r="88" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="88" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -5234,7 +5427,7 @@
       <c r="K88" s="2"/>
       <c r="L88" s="2"/>
     </row>
-    <row r="89" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="89" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -5248,7 +5441,7 @@
       <c r="K89" s="2"/>
       <c r="L89" s="2"/>
     </row>
-    <row r="90" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="90" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -5262,7 +5455,7 @@
       <c r="K90" s="2"/>
       <c r="L90" s="2"/>
     </row>
-    <row r="91" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="91" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -5276,7 +5469,7 @@
       <c r="K91" s="2"/>
       <c r="L91" s="2"/>
     </row>
-    <row r="92" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="92" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -5290,7 +5483,7 @@
       <c r="K92" s="2"/>
       <c r="L92" s="2"/>
     </row>
-    <row r="93" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="93" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -5304,7 +5497,7 @@
       <c r="K93" s="2"/>
       <c r="L93" s="2"/>
     </row>
-    <row r="94" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="94" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -5318,7 +5511,7 @@
       <c r="K94" s="2"/>
       <c r="L94" s="2"/>
     </row>
-    <row r="95" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="95" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -5332,7 +5525,7 @@
       <c r="K95" s="2"/>
       <c r="L95" s="2"/>
     </row>
-    <row r="96" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="96" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -5346,7 +5539,7 @@
       <c r="K96" s="2"/>
       <c r="L96" s="2"/>
     </row>
-    <row r="97" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="97" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -5360,7 +5553,7 @@
       <c r="K97" s="2"/>
       <c r="L97" s="2"/>
     </row>
-    <row r="98" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="98" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -5374,7 +5567,7 @@
       <c r="K98" s="2"/>
       <c r="L98" s="2"/>
     </row>
-    <row r="99" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="99" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -5388,7 +5581,7 @@
       <c r="K99" s="2"/>
       <c r="L99" s="2"/>
     </row>
-    <row r="100" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="100" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -5402,7 +5595,7 @@
       <c r="K100" s="2"/>
       <c r="L100" s="2"/>
     </row>
-    <row r="101" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="101" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -5416,7 +5609,7 @@
       <c r="K101" s="2"/>
       <c r="L101" s="2"/>
     </row>
-    <row r="102" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="102" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -5430,7 +5623,7 @@
       <c r="K102" s="2"/>
       <c r="L102" s="2"/>
     </row>
-    <row r="103" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="103" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -5444,7 +5637,7 @@
       <c r="K103" s="2"/>
       <c r="L103" s="2"/>
     </row>
-    <row r="104" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="104" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -5458,7 +5651,7 @@
       <c r="K104" s="2"/>
       <c r="L104" s="2"/>
     </row>
-    <row r="105" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="105" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -5472,7 +5665,7 @@
       <c r="K105" s="2"/>
       <c r="L105" s="2"/>
     </row>
-    <row r="106" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="106" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -5486,7 +5679,7 @@
       <c r="K106" s="2"/>
       <c r="L106" s="2"/>
     </row>
-    <row r="107" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="107" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -5500,7 +5693,7 @@
       <c r="K107" s="2"/>
       <c r="L107" s="2"/>
     </row>
-    <row r="108" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="108" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -5514,7 +5707,7 @@
       <c r="K108" s="2"/>
       <c r="L108" s="2"/>
     </row>
-    <row r="109" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="109" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -5528,7 +5721,7 @@
       <c r="K109" s="2"/>
       <c r="L109" s="2"/>
     </row>
-    <row r="110" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="110" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -5542,7 +5735,7 @@
       <c r="K110" s="2"/>
       <c r="L110" s="2"/>
     </row>
-    <row r="111" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="111" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -5556,7 +5749,7 @@
       <c r="K111" s="2"/>
       <c r="L111" s="2"/>
     </row>
-    <row r="112" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="112" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -5570,7 +5763,7 @@
       <c r="K112" s="2"/>
       <c r="L112" s="2"/>
     </row>
-    <row r="113" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="113" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -5584,7 +5777,7 @@
       <c r="K113" s="2"/>
       <c r="L113" s="2"/>
     </row>
-    <row r="114" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="114" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -5598,7 +5791,7 @@
       <c r="K114" s="2"/>
       <c r="L114" s="2"/>
     </row>
-    <row r="115" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="115" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -5612,7 +5805,7 @@
       <c r="K115" s="2"/>
       <c r="L115" s="2"/>
     </row>
-    <row r="116" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="116" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -5626,7 +5819,7 @@
       <c r="K116" s="2"/>
       <c r="L116" s="2"/>
     </row>
-    <row r="117" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="117" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -5640,7 +5833,7 @@
       <c r="K117" s="2"/>
       <c r="L117" s="2"/>
     </row>
-    <row r="118" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="118" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -5654,7 +5847,7 @@
       <c r="K118" s="2"/>
       <c r="L118" s="2"/>
     </row>
-    <row r="119" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="119" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -5668,7 +5861,7 @@
       <c r="K119" s="2"/>
       <c r="L119" s="2"/>
     </row>
-    <row r="120" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="120" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
@@ -5682,7 +5875,7 @@
       <c r="K120" s="2"/>
       <c r="L120" s="2"/>
     </row>
-    <row r="121" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="121" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A121" s="2"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
@@ -5696,7 +5889,7 @@
       <c r="K121" s="2"/>
       <c r="L121" s="2"/>
     </row>
-    <row r="122" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="122" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A122" s="2"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
@@ -5710,7 +5903,7 @@
       <c r="K122" s="2"/>
       <c r="L122" s="2"/>
     </row>
-    <row r="123" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="123" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A123" s="2"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
@@ -5724,7 +5917,7 @@
       <c r="K123" s="2"/>
       <c r="L123" s="2"/>
     </row>
-    <row r="124" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="124" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A124" s="2"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
@@ -5738,7 +5931,7 @@
       <c r="K124" s="2"/>
       <c r="L124" s="2"/>
     </row>
-    <row r="125" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="125" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A125" s="2"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
@@ -5752,7 +5945,7 @@
       <c r="K125" s="2"/>
       <c r="L125" s="2"/>
     </row>
-    <row r="126" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="126" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A126" s="2"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
@@ -5766,7 +5959,7 @@
       <c r="K126" s="2"/>
       <c r="L126" s="2"/>
     </row>
-    <row r="127" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="127" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A127" s="2"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
@@ -5780,7 +5973,7 @@
       <c r="K127" s="2"/>
       <c r="L127" s="2"/>
     </row>
-    <row r="128" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="128" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A128" s="2"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
@@ -5794,7 +5987,7 @@
       <c r="K128" s="2"/>
       <c r="L128" s="2"/>
     </row>
-    <row r="129" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="129" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A129" s="2"/>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
@@ -5808,7 +6001,7 @@
       <c r="K129" s="2"/>
       <c r="L129" s="2"/>
     </row>
-    <row r="130" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="130" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A130" s="2"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
@@ -5822,7 +6015,7 @@
       <c r="K130" s="2"/>
       <c r="L130" s="2"/>
     </row>
-    <row r="131" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="131" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A131" s="2"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
@@ -5836,7 +6029,7 @@
       <c r="K131" s="2"/>
       <c r="L131" s="2"/>
     </row>
-    <row r="132" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="132" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A132" s="2"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
@@ -5850,7 +6043,7 @@
       <c r="K132" s="2"/>
       <c r="L132" s="2"/>
     </row>
-    <row r="133" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="133" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A133" s="2"/>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>

</xml_diff>